<commit_message>
updated with GUI version
</commit_message>
<xml_diff>
--- a/projects/atm_with_excel_as_database/bank_accounts.xlsx
+++ b/projects/atm_with_excel_as_database/bank_accounts.xlsx
@@ -19,9 +19,10 @@
   <numFmts count="1">
     <numFmt formatCode="YYYY\-MM\-DD" numFmtId="164"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -41,137 +42,27 @@
       <sz val="10"/>
     </font>
     <font>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-      <color rgb="FF333333"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-      <color rgb="FF808080"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-      <color rgb="FF0000EE"/>
-      <sz val="10"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-      <color rgb="FF006600"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-      <color rgb="FF996600"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-      <color rgb="FFCC0000"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="1"/>
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -182,7 +73,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="6">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -191,75 +82,44 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="43"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="41"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="44"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="42"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="9"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle builtinId="3" name="Comma" xfId="1"/>
     <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
     <cellStyle builtinId="4" name="Currency" xfId="3"/>
     <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
     <cellStyle builtinId="5" name="Percent" xfId="5"/>
-    <cellStyle builtinId="53" name="Heading" xfId="6"/>
-    <cellStyle builtinId="53" name="Heading 1" xfId="7"/>
-    <cellStyle builtinId="53" name="Heading 2" xfId="8"/>
-    <cellStyle builtinId="53" name="Text" xfId="9"/>
-    <cellStyle builtinId="53" name="Note" xfId="10"/>
-    <cellStyle builtinId="53" name="Footnote" xfId="11"/>
-    <cellStyle builtinId="53" name="Hyperlink" xfId="12"/>
-    <cellStyle builtinId="53" name="Status" xfId="13"/>
-    <cellStyle builtinId="53" name="Good" xfId="14"/>
-    <cellStyle builtinId="53" name="Neutral" xfId="15"/>
-    <cellStyle builtinId="53" name="Bad" xfId="16"/>
-    <cellStyle builtinId="53" name="Warning" xfId="17"/>
-    <cellStyle builtinId="53" name="Error" xfId="18"/>
-    <cellStyle builtinId="53" name="Accent" xfId="19"/>
-    <cellStyle builtinId="53" name="Accent 1" xfId="20"/>
-    <cellStyle builtinId="53" name="Accent 2" xfId="21"/>
-    <cellStyle builtinId="53" name="Accent 3" xfId="22"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -553,124 +413,413 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100">
-      <selection activeCell="D17" activeCellId="0" pane="topLeft" sqref="D17"/>
+      <selection activeCell="D8" activeCellId="0" pane="topLeft" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="4" width="11.52"/>
-    <col customWidth="1" max="2" min="2" style="4" width="15.74"/>
-    <col customWidth="1" max="4" min="3" style="4" width="11.52"/>
-    <col customWidth="1" max="5" min="5" style="4" width="24.54"/>
-    <col customWidth="1" max="6" min="6" style="4" width="26.85"/>
-    <col customWidth="1" max="1025" min="7" style="4" width="11.52"/>
+    <col customWidth="1" max="1" min="1" style="5" width="11.52"/>
+    <col customWidth="1" max="2" min="2" style="5" width="15.74"/>
+    <col customWidth="1" max="3" min="3" style="5" width="14.81"/>
+    <col customWidth="1" max="4" min="4" style="5" width="11.52"/>
+    <col customWidth="1" max="5" min="5" style="5" width="24.54"/>
+    <col customWidth="1" max="6" min="6" style="5" width="26.85"/>
+    <col customWidth="1" max="1025" min="7" style="5" width="11.52"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="12.8" r="1" s="5">
-      <c r="A1" s="6" t="inlineStr">
+    <row customHeight="1" ht="12.8" r="1" s="6">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">name </t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>account_number</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Password</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>balance</t>
         </is>
       </c>
-      <c r="E1" s="6" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>last_transaction_time</t>
         </is>
       </c>
-      <c r="F1" s="6" t="inlineStr">
+      <c r="F1" s="7" t="inlineStr">
         <is>
           <t>total_transactions</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12.8" r="2" s="5">
-      <c r="A2" s="7" t="inlineStr">
+    <row customHeight="1" ht="12.8" r="2" s="6">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>ram</t>
         </is>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="8" t="n">
         <v>987654123</v>
       </c>
-      <c r="C2" s="7" t="inlineStr">
+      <c r="C2" s="8" t="inlineStr">
         <is>
           <t>Ram*1992</t>
         </is>
       </c>
-      <c r="D2" s="7" t="n">
-        <v>908868</v>
-      </c>
-      <c r="E2" s="8" t="n">
+      <c r="D2" s="8" t="n">
+        <v>900076</v>
+      </c>
+      <c r="E2" s="9" t="n">
         <v>43823</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="8" t="n">
         <v>23</v>
       </c>
     </row>
-    <row customHeight="1" ht="12.8" r="3" s="5">
-      <c r="A3" s="7" t="inlineStr">
+    <row customHeight="1" ht="12.8" r="3" s="6">
+      <c r="A3" s="8" t="inlineStr">
         <is>
           <t>ravi</t>
         </is>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="8" t="n">
         <v>987645121</v>
       </c>
-      <c r="C3" s="7" t="inlineStr">
+      <c r="C3" s="8" t="inlineStr">
         <is>
           <t>Ravi*1921</t>
         </is>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="8" t="n">
         <v>18000</v>
       </c>
-      <c r="E3" s="8" t="n">
-        <v>43821</v>
-      </c>
-      <c r="F3" s="7" t="n">
+      <c r="E3" s="9" t="n">
+        <v>43824</v>
+      </c>
+      <c r="F3" s="8" t="n">
         <v>11</v>
       </c>
     </row>
-    <row customHeight="1" ht="12.8" r="4" s="5">
-      <c r="A4" s="7" t="inlineStr">
+    <row customHeight="1" ht="12.8" r="4" s="6">
+      <c r="A4" s="8" t="inlineStr">
         <is>
           <t>gopal</t>
         </is>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="8" t="n">
         <v>987127346</v>
       </c>
-      <c r="C4" s="7" t="inlineStr">
+      <c r="C4" s="8" t="inlineStr">
         <is>
           <t>Gopal*8721</t>
         </is>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="8" t="n">
         <v>500</v>
       </c>
-      <c r="E4" s="8" t="n">
-        <v>43792</v>
-      </c>
-      <c r="F4" s="7" t="n">
+      <c r="E4" s="9" t="n">
+        <v>43825</v>
+      </c>
+      <c r="F4" s="8" t="n">
         <v>32</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="5" s="6">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Mani</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>912312324</v>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>123Mani</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>234213</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>43826</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="6" s="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>Rahul</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>932422421</v>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Pass*123</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>7400</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>43827</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="7" s="6">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Athi</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>923123132</v>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>Athi*123</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>872</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>43828</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="8" s="6">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>Abish</t>
+        </is>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>945433464</v>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>Abish*123</t>
+        </is>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>2345</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>43829</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="9" s="6">
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>Clinton</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>935232434</v>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>Clinton*123</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>2324</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>43830</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="10" s="6">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>Mosses</t>
+        </is>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>923454322</v>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>Mosses*123</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>1242</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>43831</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="11" s="6">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>Gowtham</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>923443423</v>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>Gowtham*123</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>8222</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>43832</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="12" s="6">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>ranjith</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>964322222</v>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>Ranjith*123</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>90000</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>43833</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="13" s="6">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>keerthana</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>945345334</v>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>Keerthan*123</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>80000</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <v>43834</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="14" s="6">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>nandhini</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>934534643</v>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>Nandhini*123</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>43835</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="15" s="6">
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>suriya</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>967456322</v>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>Surya*123</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>12222</v>
+      </c>
+      <c r="E15" s="9" t="n">
+        <v>43836</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="16" s="6">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>vasika</t>
+        </is>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>912355344</v>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>Vasika*123</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>39999</v>
+      </c>
+      <c r="E16" s="9" t="n">
+        <v>43837</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>